<commit_message>
Đang làm login đăng nhập phân quyền
</commit_message>
<xml_diff>
--- a/listFunction.xlsx
+++ b/listFunction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\assgnmentPhp3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A78B09-CD3B-441F-A208-2F6D9F523A88}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB1FF4A-6BA5-439A-B84D-18F9CD44777E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1335" yWindow="1020" windowWidth="15375" windowHeight="7875" xr2:uid="{11F4A3C5-2F94-492F-99D1-233B4A8DF012}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{11F4A3C5-2F94-492F-99D1-233B4A8DF012}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>STT</t>
   </si>
@@ -109,6 +109,12 @@
   </si>
   <si>
     <t>all</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Để ý phần slug sản phẩm</t>
   </si>
 </sst>
 </file>
@@ -178,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -196,6 +202,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -514,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1EDFD63-4F7D-4D08-A02C-7D38C1492053}">
   <dimension ref="G1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,6 +672,12 @@
       <c r="I12" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="J12" t="s">
+        <v>26</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="13" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G13" s="1">

</xml_diff>